<commit_message>
First Update. Exception handling and printing installed software
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\OneDrive - University of Nottingham Malaysia Campus\Future University\QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624BDE92-5094-4FEE-A51F-C1CD629A4B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B327D5-6E2F-4F59-96DD-B54254A1F3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7810" xr2:uid="{F1D96436-C3AE-40A1-9570-A8B53EAA5337}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Serial Number</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Intel® HD Graphics 4600</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7566A94C-69F7-4E7C-B583-348A1C259327}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,6 +575,32 @@
         <v>22</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>